<commit_message>
additional changes for Delivery 4
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/SicomApp.xlsx
+++ b/Popeyes.suite/Resources/SicomApp.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -49,6 +49,12 @@
     <t xml:space="preserve">LabelMealDisplayName</t>
   </si>
   <si>
+    <t xml:space="preserve">ProteinDisplayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SidesDisplayName</t>
+  </si>
+  <si>
     <t xml:space="preserve">spicysand_delivery</t>
   </si>
   <si>
@@ -73,18 +79,42 @@
     <t xml:space="preserve">Spicy Cheese, Cajun Rice Rg</t>
   </si>
   <si>
+    <t xml:space="preserve">Mac &amp; Chs Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">sideitem_delivery</t>
   </si>
   <si>
     <t xml:space="preserve">sideitem</t>
   </si>
   <si>
+    <t xml:space="preserve">Chkn Dippers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Mash &amp; Gravy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coleslaw Lg</t>
+  </si>
+  <si>
     <t xml:space="preserve">popcornshrimp_tenders_delivery</t>
   </si>
   <si>
     <t xml:space="preserve">popcornshrimp_tenders</t>
   </si>
   <si>
+    <t xml:space="preserve">LgCmb SHRMP, LgCmb SHRIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popcorn Shrimp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LgCmb SHRMP POP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mash &amp; Gravy Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">spicysand_pickup</t>
   </si>
   <si>
@@ -95,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">popcornshrimp_tenders_pickup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LgCmb SHRMP, LgCmb SHRMP</t>
   </si>
 </sst>
 </file>
@@ -306,10 +339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,6 +354,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="48.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="39.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="1" width="12.31"/>
   </cols>
   <sheetData>
@@ -352,34 +387,43 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -387,34 +431,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="I3" s="2"/>
+      <c r="J3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -422,28 +490,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -451,16 +522,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="J6" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -468,16 +551,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>